<commit_message>
data changed. one more sheet
</commit_message>
<xml_diff>
--- a/Backend/db_schema.xlsx
+++ b/Backend/db_schema.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="RawData" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="53">
   <si>
     <t xml:space="preserve">ColumnName</t>
   </si>
@@ -173,6 +174,15 @@
   </si>
   <si>
     <t xml:space="preserve">Item10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hexString</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x01ADBC1234544BCCCDDDCDAADB</t>
   </si>
 </sst>
 </file>
@@ -182,7 +192,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -212,12 +222,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -269,7 +273,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -279,10 +283,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -603,7 +603,7 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -657,7 +657,7 @@
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="2" t="n">
@@ -690,7 +690,7 @@
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="2" t="n">
@@ -791,7 +791,7 @@
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="2" t="n">
@@ -868,7 +868,7 @@
       <c r="A11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="2" t="n">
@@ -884,4 +884,102 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.33"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>